<commit_message>
just doing some tests in client code
</commit_message>
<xml_diff>
--- a/Group02LogYYMMDD.xlsx
+++ b/Group02LogYYMMDD.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="118">
   <si>
     <t xml:space="preserve">Team Name:</t>
   </si>
@@ -319,6 +319,9 @@
   </si>
   <si>
     <t xml:space="preserve">180320T14:30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">completed</t>
   </si>
   <si>
     <t xml:space="preserve">180320T09:31</t>
@@ -621,9 +624,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>202680</xdr:colOff>
+      <xdr:colOff>202320</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>203040</xdr:rowOff>
+      <xdr:rowOff>202680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -634,8 +637,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8982000" y="3060720"/>
-          <a:ext cx="202680" cy="202680"/>
+          <a:off x="8858160" y="3060720"/>
+          <a:ext cx="202320" cy="202320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -664,19 +667,19 @@
   </sheetPr>
   <dimension ref="A1:G153"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F47" activeCellId="0" sqref="F47"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E44" activeCellId="0" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.9336734693878"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="58.3163265306122"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="32.8010204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="57.6428571428571"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="32.3979591836735"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="10.3928571428571"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1378,13 +1381,15 @@
         <v>33</v>
       </c>
       <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
+      <c r="E38" s="3" t="s">
+        <v>93</v>
+      </c>
       <c r="F38" s="3"/>
       <c r="G38" s="3"/>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="12" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>22</v>
@@ -1394,16 +1399,16 @@
         <v>21</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G39" s="3"/>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="12" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>14</v>
@@ -1413,16 +1418,16 @@
         <v>22</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G40" s="3"/>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="12" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>20</v>
@@ -1435,13 +1440,13 @@
         <v>34</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="G41" s="3"/>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="12" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>32</v>
@@ -1456,13 +1461,13 @@
         <v>34</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="G42" s="3"/>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="12" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>70</v>
@@ -1474,31 +1479,33 @@
         <v>26</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="G43" s="3"/>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="12" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>32</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D44" s="3"/>
-      <c r="E44" s="3"/>
+      <c r="E44" s="3" t="s">
+        <v>93</v>
+      </c>
       <c r="F44" s="3"/>
       <c r="G44" s="3"/>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="12" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>22</v>
@@ -1508,16 +1515,16 @@
         <v>27</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="G45" s="3"/>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="12" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>14</v>
@@ -1530,13 +1537,13 @@
         <v>34</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="G46" s="3"/>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="12" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>20</v>
@@ -1544,16 +1551,16 @@
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
       <c r="E47" s="3" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="G47" s="3"/>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="12" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>22</v>
@@ -1566,13 +1573,13 @@
         <v>34</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="G48" s="3"/>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="12" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>22</v>
@@ -1587,16 +1594,16 @@
         <v>34</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="G49" s="3"/>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="12" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C50" s="3" t="s">
         <v>63</v>
@@ -1608,19 +1615,19 @@
         <v>34</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="G50" s="3"/>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="12" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>32</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D51" s="3"/>
       <c r="E51" s="3" t="s">

</xml_diff>